<commit_message>
correção dos targets com menos de 10%
</commit_message>
<xml_diff>
--- a/data/dados.xlsx
+++ b/data/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Dourado\Desktop\Programação\Insper\cdados\22-2a-cd-p1-grupo_rafaeldbo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F724A460-E850-4DFE-B0DC-013D23756551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A1412E-75D2-4360-927D-68FE1F8CFABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5612" uniqueCount="4192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5612" uniqueCount="4191">
   <si>
     <t>Categoria</t>
   </si>
@@ -11260,9 +11260,6 @@
   </si>
   <si>
     <t>O estado de Nova York anunciou oficialmente nesta quarta-feira (9) o fim da obrigatoriedade do uso de máscaras em espaços fechados, em linha com outros estados governados por democratas, diante da queda acentuada de casos de covid-19 e o cansaço da população com medidas coercitivas após quase dois anos de pandemia. A partir desta quinta-feira, […]</t>
-  </si>
-  <si>
-    <t>A proposta de fusão entre a operadora francesa de satélites Eutelsat e a britânica OneWeb ilustra a ascensão da Internet espacial de alta velocidade, destinada a atender regiões isoladas, sem redes de fibra ótica, ou cobertura móvel, sem passar por infraestruturas terrestres. – Quem são os atores? Neste mercado “em expansão”, estimado em US$ 16 […]</t>
   </si>
   <si>
     <t>Que praticar exercícios regularmente leva a uma vida mais saudável não é novidade. No entanto, uma pesquisa realizada pelo Instituto Nacional do Câncer e do Centro de Controle e Prevenção de Doenças (CDC) dos Estados Unidos indica que caminhar por apenas 10 minutos por dia pode evitar 111 mil mortes por ano apenas no país. […]</t>
@@ -13013,8 +13010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A1000" workbookViewId="0">
-      <selection activeCell="C272" sqref="C272"/>
+    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="C386" sqref="C386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13164,7 +13161,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -14824,7 +14821,7 @@
         <v>8</v>
       </c>
       <c r="F90" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -15664,7 +15661,7 @@
         <v>8</v>
       </c>
       <c r="F132" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -15684,7 +15681,7 @@
         <v>64</v>
       </c>
       <c r="F133" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -17272,7 +17269,7 @@
         <v>6</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>4188</v>
+        <v>4187</v>
       </c>
       <c r="C213" s="5" t="s">
         <v>1175</v>
@@ -20724,7 +20721,7 @@
         <v>16</v>
       </c>
       <c r="F385" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -22715,7 +22712,7 @@
         <v>488</v>
       </c>
       <c r="C485" s="5" t="s">
-        <v>4187</v>
+        <v>4186</v>
       </c>
       <c r="D485" s="4" t="s">
         <v>2406</v>
@@ -23644,7 +23641,7 @@
         <v>4</v>
       </c>
       <c r="F531" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="532" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -24284,7 +24281,7 @@
         <v>22</v>
       </c>
       <c r="F563" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="564" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -24924,7 +24921,7 @@
         <v>29</v>
       </c>
       <c r="F595" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="596" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -26824,7 +26821,7 @@
         <v>14</v>
       </c>
       <c r="F690" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="691" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -29144,7 +29141,7 @@
         <v>64</v>
       </c>
       <c r="F806" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="807" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -29184,7 +29181,7 @@
         <v>79</v>
       </c>
       <c r="F808" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="809" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -30224,7 +30221,7 @@
         <v>65</v>
       </c>
       <c r="F860" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="861" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -31364,7 +31361,7 @@
         <v>24</v>
       </c>
       <c r="F917" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="918" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -32258,7 +32255,7 @@
         <v>3713</v>
       </c>
       <c r="D962" s="4" t="s">
-        <v>4149</v>
+        <v>4148</v>
       </c>
       <c r="E962" s="4">
         <v>15</v>
@@ -32278,7 +32275,7 @@
         <v>3714</v>
       </c>
       <c r="D963" s="4" t="s">
-        <v>4150</v>
+        <v>4149</v>
       </c>
       <c r="E963" s="4">
         <v>40</v>
@@ -32298,7 +32295,7 @@
         <v>3715</v>
       </c>
       <c r="D964" s="4" t="s">
-        <v>4151</v>
+        <v>4150</v>
       </c>
       <c r="E964" s="4">
         <v>21</v>
@@ -32318,7 +32315,7 @@
         <v>3716</v>
       </c>
       <c r="D965" s="4" t="s">
-        <v>4152</v>
+        <v>4151</v>
       </c>
       <c r="E965" s="4">
         <v>5</v>
@@ -32338,7 +32335,7 @@
         <v>3717</v>
       </c>
       <c r="D966" s="4" t="s">
-        <v>4153</v>
+        <v>4152</v>
       </c>
       <c r="E966" s="4">
         <v>58</v>
@@ -32358,7 +32355,7 @@
         <v>3718</v>
       </c>
       <c r="D967" s="4" t="s">
-        <v>4154</v>
+        <v>4153</v>
       </c>
       <c r="E967" s="4">
         <v>55</v>
@@ -32378,7 +32375,7 @@
         <v>3719</v>
       </c>
       <c r="D968" s="4" t="s">
-        <v>4155</v>
+        <v>4154</v>
       </c>
       <c r="E968" s="4">
         <v>20</v>
@@ -32398,7 +32395,7 @@
         <v>3720</v>
       </c>
       <c r="D969" s="4" t="s">
-        <v>4156</v>
+        <v>4155</v>
       </c>
       <c r="E969" s="4">
         <v>50</v>
@@ -32418,7 +32415,7 @@
         <v>3721</v>
       </c>
       <c r="D970" s="4" t="s">
-        <v>4157</v>
+        <v>4156</v>
       </c>
       <c r="E970" s="4">
         <v>8</v>
@@ -32438,7 +32435,7 @@
         <v>3722</v>
       </c>
       <c r="D971" s="4" t="s">
-        <v>4158</v>
+        <v>4157</v>
       </c>
       <c r="E971" s="4">
         <v>73</v>
@@ -32458,7 +32455,7 @@
         <v>3723</v>
       </c>
       <c r="D972" s="4" t="s">
-        <v>4159</v>
+        <v>4158</v>
       </c>
       <c r="E972" s="4">
         <v>32</v>
@@ -32478,7 +32475,7 @@
         <v>3724</v>
       </c>
       <c r="D973" s="4" t="s">
-        <v>4160</v>
+        <v>4159</v>
       </c>
       <c r="E973" s="4">
         <v>56</v>
@@ -32498,7 +32495,7 @@
         <v>3725</v>
       </c>
       <c r="D974" s="4" t="s">
-        <v>4161</v>
+        <v>4160</v>
       </c>
       <c r="E974" s="4">
         <v>25</v>
@@ -32518,7 +32515,7 @@
         <v>3726</v>
       </c>
       <c r="D975" s="4" t="s">
-        <v>4162</v>
+        <v>4161</v>
       </c>
       <c r="E975" s="4">
         <v>55</v>
@@ -32538,7 +32535,7 @@
         <v>3727</v>
       </c>
       <c r="D976" s="4" t="s">
-        <v>4163</v>
+        <v>4162</v>
       </c>
       <c r="E976" s="4">
         <v>58</v>
@@ -32558,7 +32555,7 @@
         <v>3728</v>
       </c>
       <c r="D977" s="4" t="s">
-        <v>4148</v>
+        <v>4147</v>
       </c>
       <c r="E977" s="4">
         <v>48</v>
@@ -32578,7 +32575,7 @@
         <v>3729</v>
       </c>
       <c r="D978" s="4" t="s">
-        <v>4164</v>
+        <v>4163</v>
       </c>
       <c r="E978" s="4">
         <v>55</v>
@@ -32598,7 +32595,7 @@
         <v>3730</v>
       </c>
       <c r="D979" s="4" t="s">
-        <v>4165</v>
+        <v>4164</v>
       </c>
       <c r="E979" s="4">
         <v>43</v>
@@ -32618,7 +32615,7 @@
         <v>3731</v>
       </c>
       <c r="D980" s="4" t="s">
-        <v>4166</v>
+        <v>4165</v>
       </c>
       <c r="E980" s="4">
         <v>9</v>
@@ -32638,7 +32635,7 @@
         <v>3732</v>
       </c>
       <c r="D981" s="4" t="s">
-        <v>4167</v>
+        <v>4166</v>
       </c>
       <c r="E981" s="4">
         <v>10</v>
@@ -32658,7 +32655,7 @@
         <v>3733</v>
       </c>
       <c r="D982" s="4" t="s">
-        <v>4168</v>
+        <v>4167</v>
       </c>
       <c r="E982" s="4">
         <v>62</v>
@@ -32678,7 +32675,7 @@
         <v>3734</v>
       </c>
       <c r="D983" s="4" t="s">
-        <v>4169</v>
+        <v>4168</v>
       </c>
       <c r="E983" s="4">
         <v>28</v>
@@ -32698,13 +32695,13 @@
         <v>3735</v>
       </c>
       <c r="D984" s="4" t="s">
-        <v>4170</v>
+        <v>4169</v>
       </c>
       <c r="E984" s="4">
         <v>66</v>
       </c>
       <c r="F984" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="985" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -32718,7 +32715,7 @@
         <v>3736</v>
       </c>
       <c r="D985" s="4" t="s">
-        <v>4171</v>
+        <v>4170</v>
       </c>
       <c r="E985" s="4">
         <v>59</v>
@@ -32738,7 +32735,7 @@
         <v>3737</v>
       </c>
       <c r="D986" s="4" t="s">
-        <v>4172</v>
+        <v>4171</v>
       </c>
       <c r="E986" s="4">
         <v>1</v>
@@ -32758,7 +32755,7 @@
         <v>3738</v>
       </c>
       <c r="D987" s="4" t="s">
-        <v>4173</v>
+        <v>4172</v>
       </c>
       <c r="E987" s="4">
         <v>54</v>
@@ -32778,7 +32775,7 @@
         <v>3739</v>
       </c>
       <c r="D988" s="4" t="s">
-        <v>4174</v>
+        <v>4173</v>
       </c>
       <c r="E988" s="4">
         <v>46</v>
@@ -32798,7 +32795,7 @@
         <v>3740</v>
       </c>
       <c r="D989" s="4" t="s">
-        <v>4175</v>
+        <v>4174</v>
       </c>
       <c r="E989" s="4">
         <v>10</v>
@@ -32818,7 +32815,7 @@
         <v>3741</v>
       </c>
       <c r="D990" s="4" t="s">
-        <v>4176</v>
+        <v>4175</v>
       </c>
       <c r="E990" s="4">
         <v>36</v>
@@ -32838,7 +32835,7 @@
         <v>3742</v>
       </c>
       <c r="D991" s="4" t="s">
-        <v>4177</v>
+        <v>4176</v>
       </c>
       <c r="E991" s="4">
         <v>4</v>
@@ -32858,7 +32855,7 @@
         <v>3743</v>
       </c>
       <c r="D992" s="4" t="s">
-        <v>4178</v>
+        <v>4177</v>
       </c>
       <c r="E992" s="4">
         <v>62</v>
@@ -32878,7 +32875,7 @@
         <v>3744</v>
       </c>
       <c r="D993" s="4" t="s">
-        <v>4179</v>
+        <v>4178</v>
       </c>
       <c r="E993" s="4">
         <v>17</v>
@@ -32898,7 +32895,7 @@
         <v>3745</v>
       </c>
       <c r="D994" s="4" t="s">
-        <v>4180</v>
+        <v>4179</v>
       </c>
       <c r="E994" s="4">
         <v>50</v>
@@ -32915,10 +32912,10 @@
         <v>3310</v>
       </c>
       <c r="C995" s="5" t="s">
-        <v>3746</v>
+        <v>3745</v>
       </c>
       <c r="D995" s="4" t="s">
-        <v>4181</v>
+        <v>4180</v>
       </c>
       <c r="E995" s="4">
         <v>10</v>
@@ -32935,10 +32932,10 @@
         <v>3311</v>
       </c>
       <c r="C996" s="5" t="s">
-        <v>3747</v>
+        <v>3746</v>
       </c>
       <c r="D996" s="4" t="s">
-        <v>4182</v>
+        <v>4181</v>
       </c>
       <c r="E996" s="4">
         <v>51</v>
@@ -32955,10 +32952,10 @@
         <v>3312</v>
       </c>
       <c r="C997" s="5" t="s">
-        <v>3748</v>
+        <v>3747</v>
       </c>
       <c r="D997" s="4" t="s">
-        <v>4183</v>
+        <v>4182</v>
       </c>
       <c r="E997" s="4">
         <v>7</v>
@@ -32975,10 +32972,10 @@
         <v>3313</v>
       </c>
       <c r="C998" s="5" t="s">
-        <v>3749</v>
+        <v>3748</v>
       </c>
       <c r="D998" s="4" t="s">
-        <v>4184</v>
+        <v>4183</v>
       </c>
       <c r="E998" s="4">
         <v>24</v>
@@ -32995,10 +32992,10 @@
         <v>3314</v>
       </c>
       <c r="C999" s="5" t="s">
-        <v>3750</v>
+        <v>3749</v>
       </c>
       <c r="D999" s="4" t="s">
-        <v>4185</v>
+        <v>4184</v>
       </c>
       <c r="E999" s="4">
         <v>11</v>
@@ -33015,10 +33012,10 @@
         <v>3315</v>
       </c>
       <c r="C1000" s="5" t="s">
-        <v>3751</v>
+        <v>3750</v>
       </c>
       <c r="D1000" s="4" t="s">
-        <v>4186</v>
+        <v>4185</v>
       </c>
       <c r="E1000" s="4">
         <v>3</v>
@@ -33032,13 +33029,13 @@
         <v>6</v>
       </c>
       <c r="B1001" s="5" t="s">
+        <v>4188</v>
+      </c>
+      <c r="C1001" s="5" t="s">
         <v>4189</v>
       </c>
-      <c r="C1001" s="5" t="s">
+      <c r="D1001" s="5" t="s">
         <v>4190</v>
-      </c>
-      <c r="D1001" s="5" t="s">
-        <v>4191</v>
       </c>
       <c r="E1001" s="5">
         <v>77</v>
@@ -33057,7 +33054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
+    <sheetView topLeftCell="A393" workbookViewId="0">
       <selection activeCell="B407" sqref="B407"/>
     </sheetView>
   </sheetViews>
@@ -33101,7 +33098,7 @@
         <v>3316</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>3752</v>
+        <v>3751</v>
       </c>
       <c r="E2" s="4">
         <v>11</v>
@@ -33121,7 +33118,7 @@
         <v>3317</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>3753</v>
+        <v>3752</v>
       </c>
       <c r="E3" s="4">
         <v>78</v>
@@ -33141,7 +33138,7 @@
         <v>3318</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>3754</v>
+        <v>3753</v>
       </c>
       <c r="E4" s="4">
         <v>35</v>
@@ -33161,7 +33158,7 @@
         <v>3319</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="E5" s="4">
         <v>53</v>
@@ -33181,7 +33178,7 @@
         <v>3320</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>3756</v>
+        <v>3755</v>
       </c>
       <c r="E6" s="4">
         <v>64</v>
@@ -33201,7 +33198,7 @@
         <v>3321</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>3757</v>
+        <v>3756</v>
       </c>
       <c r="E7" s="4">
         <v>15</v>
@@ -33221,7 +33218,7 @@
         <v>3322</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>3758</v>
+        <v>3757</v>
       </c>
       <c r="E8" s="4">
         <v>33</v>
@@ -33241,7 +33238,7 @@
         <v>3323</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>3759</v>
+        <v>3758</v>
       </c>
       <c r="E9" s="4">
         <v>71</v>
@@ -33261,7 +33258,7 @@
         <v>3324</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>3760</v>
+        <v>3759</v>
       </c>
       <c r="E10" s="4">
         <v>63</v>
@@ -33281,7 +33278,7 @@
         <v>3325</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>3761</v>
+        <v>3760</v>
       </c>
       <c r="E11" s="4">
         <v>11</v>
@@ -33301,7 +33298,7 @@
         <v>3326</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>3762</v>
+        <v>3761</v>
       </c>
       <c r="E12" s="4">
         <v>39</v>
@@ -33321,7 +33318,7 @@
         <v>3327</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>3763</v>
+        <v>3762</v>
       </c>
       <c r="E13" s="4">
         <v>33</v>
@@ -33341,7 +33338,7 @@
         <v>3328</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>3764</v>
+        <v>3763</v>
       </c>
       <c r="E14" s="4">
         <v>43</v>
@@ -33361,7 +33358,7 @@
         <v>3329</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>3765</v>
+        <v>3764</v>
       </c>
       <c r="E15" s="4">
         <v>44</v>
@@ -33381,7 +33378,7 @@
         <v>3330</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>3766</v>
+        <v>3765</v>
       </c>
       <c r="E16" s="4">
         <v>62</v>
@@ -33401,7 +33398,7 @@
         <v>3331</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
       <c r="E17" s="4">
         <v>13</v>
@@ -33421,7 +33418,7 @@
         <v>3332</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>3768</v>
+        <v>3767</v>
       </c>
       <c r="E18" s="4">
         <v>16</v>
@@ -33441,7 +33438,7 @@
         <v>3333</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>3769</v>
+        <v>3768</v>
       </c>
       <c r="E19" s="4">
         <v>41</v>
@@ -33461,7 +33458,7 @@
         <v>3334</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>3770</v>
+        <v>3769</v>
       </c>
       <c r="E20" s="4">
         <v>72</v>
@@ -33481,7 +33478,7 @@
         <v>3335</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>3771</v>
+        <v>3770</v>
       </c>
       <c r="E21" s="4">
         <v>22</v>
@@ -33501,7 +33498,7 @@
         <v>3336</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>3772</v>
+        <v>3771</v>
       </c>
       <c r="E22" s="4">
         <v>75</v>
@@ -33521,7 +33518,7 @@
         <v>3337</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>3773</v>
+        <v>3772</v>
       </c>
       <c r="E23" s="4">
         <v>77</v>
@@ -33541,7 +33538,7 @@
         <v>3338</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>3774</v>
+        <v>3773</v>
       </c>
       <c r="E24" s="4">
         <v>11</v>
@@ -33561,7 +33558,7 @@
         <v>3339</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>3775</v>
+        <v>3774</v>
       </c>
       <c r="E25" s="4">
         <v>76</v>
@@ -33581,7 +33578,7 @@
         <v>3340</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>3776</v>
+        <v>3775</v>
       </c>
       <c r="E26" s="4">
         <v>3</v>
@@ -33601,7 +33598,7 @@
         <v>3341</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>3777</v>
+        <v>3776</v>
       </c>
       <c r="E27" s="4">
         <v>62</v>
@@ -33621,7 +33618,7 @@
         <v>3342</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>3778</v>
+        <v>3777</v>
       </c>
       <c r="E28" s="4">
         <v>4</v>
@@ -33641,7 +33638,7 @@
         <v>3343</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>3779</v>
+        <v>3778</v>
       </c>
       <c r="E29" s="4">
         <v>18</v>
@@ -33661,7 +33658,7 @@
         <v>3344</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>3780</v>
+        <v>3779</v>
       </c>
       <c r="E30" s="4">
         <v>75</v>
@@ -33681,7 +33678,7 @@
         <v>3345</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>3781</v>
+        <v>3780</v>
       </c>
       <c r="E31" s="4">
         <v>34</v>
@@ -33701,7 +33698,7 @@
         <v>3346</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>3782</v>
+        <v>3781</v>
       </c>
       <c r="E32" s="4">
         <v>73</v>
@@ -33721,7 +33718,7 @@
         <v>3347</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>3783</v>
+        <v>3782</v>
       </c>
       <c r="E33" s="4">
         <v>75</v>
@@ -33741,7 +33738,7 @@
         <v>3348</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>3784</v>
+        <v>3783</v>
       </c>
       <c r="E34" s="4">
         <v>58</v>
@@ -33761,7 +33758,7 @@
         <v>3349</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>3785</v>
+        <v>3784</v>
       </c>
       <c r="E35" s="4">
         <v>26</v>
@@ -33781,7 +33778,7 @@
         <v>3350</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>3786</v>
+        <v>3785</v>
       </c>
       <c r="E36" s="4">
         <v>20</v>
@@ -33801,7 +33798,7 @@
         <v>3351</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>3787</v>
+        <v>3786</v>
       </c>
       <c r="E37" s="4">
         <v>15</v>
@@ -33821,7 +33818,7 @@
         <v>3352</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>3788</v>
+        <v>3787</v>
       </c>
       <c r="E38" s="4">
         <v>41</v>
@@ -33841,7 +33838,7 @@
         <v>3353</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>3789</v>
+        <v>3788</v>
       </c>
       <c r="E39" s="4">
         <v>65</v>
@@ -33861,7 +33858,7 @@
         <v>3354</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>3790</v>
+        <v>3789</v>
       </c>
       <c r="E40" s="4">
         <v>76</v>
@@ -33881,7 +33878,7 @@
         <v>3355</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
       <c r="E41" s="4">
         <v>49</v>
@@ -33901,7 +33898,7 @@
         <v>3356</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="E42" s="4">
         <v>65</v>
@@ -33921,7 +33918,7 @@
         <v>3357</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="E43" s="4">
         <v>16</v>
@@ -33941,7 +33938,7 @@
         <v>3358</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="E44" s="4">
         <v>67</v>
@@ -33961,7 +33958,7 @@
         <v>3359</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
       <c r="E45" s="4">
         <v>71</v>
@@ -33981,7 +33978,7 @@
         <v>3360</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="E46" s="4">
         <v>60</v>
@@ -34001,7 +33998,7 @@
         <v>3361</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
       <c r="E47" s="4">
         <v>14</v>
@@ -34021,7 +34018,7 @@
         <v>3362</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="E48" s="4">
         <v>18</v>
@@ -34041,7 +34038,7 @@
         <v>3363</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="E49" s="4">
         <v>34</v>
@@ -34061,7 +34058,7 @@
         <v>3364</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>3800</v>
+        <v>3799</v>
       </c>
       <c r="E50" s="4">
         <v>46</v>
@@ -34081,7 +34078,7 @@
         <v>3365</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
       <c r="E51" s="4">
         <v>53</v>
@@ -34101,7 +34098,7 @@
         <v>3366</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="E52" s="4">
         <v>10</v>
@@ -34141,7 +34138,7 @@
         <v>3368</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
       <c r="E54" s="4">
         <v>27</v>
@@ -34161,7 +34158,7 @@
         <v>3369</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="E55" s="4">
         <v>70</v>
@@ -34181,7 +34178,7 @@
         <v>3370</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
       <c r="E56" s="4">
         <v>38</v>
@@ -34201,7 +34198,7 @@
         <v>3371</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="E57" s="4">
         <v>39</v>
@@ -34221,7 +34218,7 @@
         <v>3372</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
       <c r="E58" s="4">
         <v>49</v>
@@ -34241,7 +34238,7 @@
         <v>3373</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="E59" s="4">
         <v>67</v>
@@ -34261,7 +34258,7 @@
         <v>3374</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
       <c r="E60" s="4">
         <v>1</v>
@@ -34281,7 +34278,7 @@
         <v>3375</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="E61" s="4">
         <v>26</v>
@@ -34301,7 +34298,7 @@
         <v>3376</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
       <c r="E62" s="4">
         <v>69</v>
@@ -34321,7 +34318,7 @@
         <v>3377</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="E63" s="4">
         <v>74</v>
@@ -34341,7 +34338,7 @@
         <v>3378</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="E64" s="4">
         <v>33</v>
@@ -34361,7 +34358,7 @@
         <v>3379</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="E65" s="4">
         <v>80</v>
@@ -34381,7 +34378,7 @@
         <v>3380</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="E66" s="4">
         <v>62</v>
@@ -34401,7 +34398,7 @@
         <v>3381</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="E67" s="4">
         <v>20</v>
@@ -34421,7 +34418,7 @@
         <v>3382</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>3817</v>
+        <v>3816</v>
       </c>
       <c r="E68" s="4">
         <v>27</v>
@@ -34441,7 +34438,7 @@
         <v>3383</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>3818</v>
+        <v>3817</v>
       </c>
       <c r="E69" s="4">
         <v>32</v>
@@ -34461,7 +34458,7 @@
         <v>3384</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="E70" s="4">
         <v>65</v>
@@ -34481,7 +34478,7 @@
         <v>3385</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>3820</v>
+        <v>3819</v>
       </c>
       <c r="E71" s="4">
         <v>37</v>
@@ -34501,7 +34498,7 @@
         <v>3386</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>3821</v>
+        <v>3820</v>
       </c>
       <c r="E72" s="4">
         <v>30</v>
@@ -34521,7 +34518,7 @@
         <v>3387</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>3822</v>
+        <v>3821</v>
       </c>
       <c r="E73" s="4">
         <v>35</v>
@@ -34541,7 +34538,7 @@
         <v>3388</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>3823</v>
+        <v>3822</v>
       </c>
       <c r="E74" s="4">
         <v>2</v>
@@ -34561,7 +34558,7 @@
         <v>3389</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>3824</v>
+        <v>3823</v>
       </c>
       <c r="E75" s="4">
         <v>42</v>
@@ -34581,7 +34578,7 @@
         <v>3390</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>3825</v>
+        <v>3824</v>
       </c>
       <c r="E76" s="4">
         <v>65</v>
@@ -34601,7 +34598,7 @@
         <v>3391</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>3826</v>
+        <v>3825</v>
       </c>
       <c r="E77" s="4">
         <v>31</v>
@@ -34621,7 +34618,7 @@
         <v>3392</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="E78" s="4">
         <v>37</v>
@@ -34641,7 +34638,7 @@
         <v>3393</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>3828</v>
+        <v>3827</v>
       </c>
       <c r="E79" s="4">
         <v>37</v>
@@ -34661,7 +34658,7 @@
         <v>3394</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>3829</v>
+        <v>3828</v>
       </c>
       <c r="E80" s="4">
         <v>33</v>
@@ -34681,7 +34678,7 @@
         <v>3395</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>3830</v>
+        <v>3829</v>
       </c>
       <c r="E81" s="4">
         <v>48</v>
@@ -34701,7 +34698,7 @@
         <v>3396</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>3831</v>
+        <v>3830</v>
       </c>
       <c r="E82" s="4">
         <v>7</v>
@@ -34721,7 +34718,7 @@
         <v>3397</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>3832</v>
+        <v>3831</v>
       </c>
       <c r="E83" s="4">
         <v>21</v>
@@ -34741,7 +34738,7 @@
         <v>3398</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>3833</v>
+        <v>3832</v>
       </c>
       <c r="E84" s="4">
         <v>70</v>
@@ -34761,7 +34758,7 @@
         <v>3399</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="E85" s="4">
         <v>48</v>
@@ -34781,7 +34778,7 @@
         <v>3400</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="E86" s="4">
         <v>34</v>
@@ -34801,7 +34798,7 @@
         <v>3401</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="E87" s="4">
         <v>71</v>
@@ -34821,7 +34818,7 @@
         <v>3402</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="E88" s="4">
         <v>36</v>
@@ -34841,7 +34838,7 @@
         <v>3403</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="E89" s="4">
         <v>64</v>
@@ -34861,7 +34858,7 @@
         <v>3404</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="E90" s="4">
         <v>31</v>
@@ -34881,7 +34878,7 @@
         <v>3405</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>3840</v>
+        <v>3839</v>
       </c>
       <c r="E91" s="4">
         <v>6</v>
@@ -34901,7 +34898,7 @@
         <v>3406</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>3841</v>
+        <v>3840</v>
       </c>
       <c r="E92" s="4">
         <v>57</v>
@@ -34921,7 +34918,7 @@
         <v>3407</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>3842</v>
+        <v>3841</v>
       </c>
       <c r="E93" s="4">
         <v>48</v>
@@ -34941,7 +34938,7 @@
         <v>3408</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>3843</v>
+        <v>3842</v>
       </c>
       <c r="E94" s="4">
         <v>34</v>
@@ -34961,7 +34958,7 @@
         <v>3409</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>3844</v>
+        <v>3843</v>
       </c>
       <c r="E95" s="4">
         <v>52</v>
@@ -34981,7 +34978,7 @@
         <v>3410</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>3845</v>
+        <v>3844</v>
       </c>
       <c r="E96" s="4">
         <v>67</v>
@@ -35001,7 +34998,7 @@
         <v>3411</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
       <c r="E97" s="4">
         <v>16</v>
@@ -35021,7 +35018,7 @@
         <v>3412</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>3847</v>
+        <v>3846</v>
       </c>
       <c r="E98" s="4">
         <v>25</v>
@@ -35041,7 +35038,7 @@
         <v>3413</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>3848</v>
+        <v>3847</v>
       </c>
       <c r="E99" s="4">
         <v>55</v>
@@ -35061,7 +35058,7 @@
         <v>3414</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>3849</v>
+        <v>3848</v>
       </c>
       <c r="E100" s="4">
         <v>41</v>
@@ -35081,7 +35078,7 @@
         <v>3415</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="E101" s="4">
         <v>16</v>
@@ -35101,7 +35098,7 @@
         <v>3416</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>3851</v>
+        <v>3850</v>
       </c>
       <c r="E102" s="4">
         <v>28</v>
@@ -35121,7 +35118,7 @@
         <v>3417</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>3852</v>
+        <v>3851</v>
       </c>
       <c r="E103" s="4">
         <v>50</v>
@@ -35141,7 +35138,7 @@
         <v>3418</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>3853</v>
+        <v>3852</v>
       </c>
       <c r="E104" s="4">
         <v>64</v>
@@ -35161,7 +35158,7 @@
         <v>3419</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>3854</v>
+        <v>3853</v>
       </c>
       <c r="E105" s="4">
         <v>30</v>
@@ -35181,7 +35178,7 @@
         <v>3420</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>3855</v>
+        <v>3854</v>
       </c>
       <c r="E106" s="4">
         <v>19</v>
@@ -35201,7 +35198,7 @@
         <v>3421</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>3856</v>
+        <v>3855</v>
       </c>
       <c r="E107" s="4">
         <v>12</v>
@@ -35221,7 +35218,7 @@
         <v>3422</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>3857</v>
+        <v>3856</v>
       </c>
       <c r="E108" s="4">
         <v>24</v>
@@ -35241,7 +35238,7 @@
         <v>3423</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>3858</v>
+        <v>3857</v>
       </c>
       <c r="E109" s="4">
         <v>59</v>
@@ -35261,7 +35258,7 @@
         <v>3424</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>3859</v>
+        <v>3858</v>
       </c>
       <c r="E110" s="4">
         <v>74</v>
@@ -35281,7 +35278,7 @@
         <v>3425</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="E111" s="4">
         <v>12</v>
@@ -35301,7 +35298,7 @@
         <v>3426</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>3861</v>
+        <v>3860</v>
       </c>
       <c r="E112" s="4">
         <v>25</v>
@@ -35321,7 +35318,7 @@
         <v>3427</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>3862</v>
+        <v>3861</v>
       </c>
       <c r="E113" s="4">
         <v>35</v>
@@ -35341,7 +35338,7 @@
         <v>3428</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>3863</v>
+        <v>3862</v>
       </c>
       <c r="E114" s="4">
         <v>69</v>
@@ -35361,7 +35358,7 @@
         <v>3429</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>3864</v>
+        <v>3863</v>
       </c>
       <c r="E115" s="4">
         <v>24</v>
@@ -35381,7 +35378,7 @@
         <v>3430</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>3865</v>
+        <v>3864</v>
       </c>
       <c r="E116" s="4">
         <v>13</v>
@@ -35401,7 +35398,7 @@
         <v>3431</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>3866</v>
+        <v>3865</v>
       </c>
       <c r="E117" s="4">
         <v>41</v>
@@ -35421,7 +35418,7 @@
         <v>3432</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>3867</v>
+        <v>3866</v>
       </c>
       <c r="E118" s="4">
         <v>61</v>
@@ -35441,7 +35438,7 @@
         <v>3433</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>3868</v>
+        <v>3867</v>
       </c>
       <c r="E119" s="4">
         <v>70</v>
@@ -35461,7 +35458,7 @@
         <v>3434</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>3869</v>
+        <v>3868</v>
       </c>
       <c r="E120" s="4">
         <v>49</v>
@@ -35481,7 +35478,7 @@
         <v>3435</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>3870</v>
+        <v>3869</v>
       </c>
       <c r="E121" s="4">
         <v>61</v>
@@ -35501,7 +35498,7 @@
         <v>3436</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>3871</v>
+        <v>3870</v>
       </c>
       <c r="E122" s="4">
         <v>29</v>
@@ -35521,7 +35518,7 @@
         <v>3437</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>3872</v>
+        <v>3871</v>
       </c>
       <c r="E123" s="4">
         <v>11</v>
@@ -35541,7 +35538,7 @@
         <v>3438</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="E124" s="4">
         <v>8</v>
@@ -35561,7 +35558,7 @@
         <v>3439</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>3874</v>
+        <v>3873</v>
       </c>
       <c r="E125" s="4">
         <v>51</v>
@@ -35581,7 +35578,7 @@
         <v>3440</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>3875</v>
+        <v>3874</v>
       </c>
       <c r="E126" s="4">
         <v>9</v>
@@ -35601,7 +35598,7 @@
         <v>3441</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>3876</v>
+        <v>3875</v>
       </c>
       <c r="E127" s="4">
         <v>49</v>
@@ -35621,7 +35618,7 @@
         <v>3442</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
       <c r="E128" s="4">
         <v>31</v>
@@ -35641,7 +35638,7 @@
         <v>3443</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>3878</v>
+        <v>3877</v>
       </c>
       <c r="E129" s="4">
         <v>49</v>
@@ -35661,7 +35658,7 @@
         <v>3444</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>3879</v>
+        <v>3878</v>
       </c>
       <c r="E130" s="4">
         <v>64</v>
@@ -35681,7 +35678,7 @@
         <v>3445</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>3880</v>
+        <v>3879</v>
       </c>
       <c r="E131" s="4">
         <v>79</v>
@@ -35701,7 +35698,7 @@
         <v>3446</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>3881</v>
+        <v>3880</v>
       </c>
       <c r="E132" s="4">
         <v>3</v>
@@ -35721,7 +35718,7 @@
         <v>3447</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
       <c r="E133" s="4">
         <v>22</v>
@@ -35741,7 +35738,7 @@
         <v>3448</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>3883</v>
+        <v>3882</v>
       </c>
       <c r="E134" s="4">
         <v>59</v>
@@ -35761,7 +35758,7 @@
         <v>3449</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="E135" s="4">
         <v>28</v>
@@ -35781,7 +35778,7 @@
         <v>3450</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="E136" s="4">
         <v>21</v>
@@ -35801,7 +35798,7 @@
         <v>3451</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="E137" s="4">
         <v>14</v>
@@ -35821,7 +35818,7 @@
         <v>3452</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="E138" s="4">
         <v>48</v>
@@ -35841,7 +35838,7 @@
         <v>3453</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>3888</v>
+        <v>3887</v>
       </c>
       <c r="E139" s="4">
         <v>42</v>
@@ -35861,7 +35858,7 @@
         <v>3454</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>3889</v>
+        <v>3888</v>
       </c>
       <c r="E140" s="4">
         <v>18</v>
@@ -35881,7 +35878,7 @@
         <v>3455</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="E141" s="4">
         <v>49</v>
@@ -35901,7 +35898,7 @@
         <v>3456</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>3891</v>
+        <v>3890</v>
       </c>
       <c r="E142" s="4">
         <v>22</v>
@@ -35921,7 +35918,7 @@
         <v>3457</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>3892</v>
+        <v>3891</v>
       </c>
       <c r="E143" s="4">
         <v>54</v>
@@ -35941,7 +35938,7 @@
         <v>3458</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
       <c r="E144" s="4">
         <v>42</v>
@@ -35961,7 +35958,7 @@
         <v>3459</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="E145" s="4">
         <v>78</v>
@@ -35981,7 +35978,7 @@
         <v>3460</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>3895</v>
+        <v>3894</v>
       </c>
       <c r="E146" s="4">
         <v>37</v>
@@ -36001,7 +35998,7 @@
         <v>3461</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>3896</v>
+        <v>3895</v>
       </c>
       <c r="E147" s="4">
         <v>11</v>
@@ -36021,7 +36018,7 @@
         <v>3462</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>3897</v>
+        <v>3896</v>
       </c>
       <c r="E148" s="4">
         <v>40</v>
@@ -36041,7 +36038,7 @@
         <v>3463</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="E149" s="4">
         <v>37</v>
@@ -36061,7 +36058,7 @@
         <v>3464</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="E150" s="4">
         <v>72</v>
@@ -36081,7 +36078,7 @@
         <v>3465</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="E151" s="4">
         <v>53</v>
@@ -36101,7 +36098,7 @@
         <v>3466</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>3901</v>
+        <v>3900</v>
       </c>
       <c r="E152" s="4">
         <v>43</v>
@@ -36121,7 +36118,7 @@
         <v>3467</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>3902</v>
+        <v>3901</v>
       </c>
       <c r="E153" s="4">
         <v>35</v>
@@ -36141,7 +36138,7 @@
         <v>3468</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>3903</v>
+        <v>3902</v>
       </c>
       <c r="E154" s="4">
         <v>15</v>
@@ -36161,7 +36158,7 @@
         <v>3469</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>3904</v>
+        <v>3903</v>
       </c>
       <c r="E155" s="4">
         <v>5</v>
@@ -36181,7 +36178,7 @@
         <v>3470</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>3905</v>
+        <v>3904</v>
       </c>
       <c r="E156" s="4">
         <v>23</v>
@@ -36201,7 +36198,7 @@
         <v>3471</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>3906</v>
+        <v>3905</v>
       </c>
       <c r="E157" s="4">
         <v>21</v>
@@ -36221,7 +36218,7 @@
         <v>3472</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>3907</v>
+        <v>3906</v>
       </c>
       <c r="E158" s="4">
         <v>76</v>
@@ -36241,7 +36238,7 @@
         <v>3473</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>3908</v>
+        <v>3907</v>
       </c>
       <c r="E159" s="4">
         <v>49</v>
@@ -36261,7 +36258,7 @@
         <v>3474</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>3909</v>
+        <v>3908</v>
       </c>
       <c r="E160" s="4">
         <v>13</v>
@@ -36281,7 +36278,7 @@
         <v>3475</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>3910</v>
+        <v>3909</v>
       </c>
       <c r="E161" s="4">
         <v>69</v>
@@ -36301,7 +36298,7 @@
         <v>3476</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>3911</v>
+        <v>3910</v>
       </c>
       <c r="E162" s="4">
         <v>77</v>
@@ -36321,7 +36318,7 @@
         <v>3477</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>3912</v>
+        <v>3911</v>
       </c>
       <c r="E163" s="4">
         <v>38</v>
@@ -36341,7 +36338,7 @@
         <v>3478</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>3913</v>
+        <v>3912</v>
       </c>
       <c r="E164" s="4">
         <v>56</v>
@@ -36361,7 +36358,7 @@
         <v>3479</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>3914</v>
+        <v>3913</v>
       </c>
       <c r="E165" s="4">
         <v>44</v>
@@ -36381,7 +36378,7 @@
         <v>3480</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>3915</v>
+        <v>3914</v>
       </c>
       <c r="E166" s="4">
         <v>58</v>
@@ -36401,7 +36398,7 @@
         <v>3481</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>3916</v>
+        <v>3915</v>
       </c>
       <c r="E167" s="4">
         <v>78</v>
@@ -36421,7 +36418,7 @@
         <v>3482</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>3917</v>
+        <v>3916</v>
       </c>
       <c r="E168" s="4">
         <v>77</v>
@@ -36441,7 +36438,7 @@
         <v>3483</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>3918</v>
+        <v>3917</v>
       </c>
       <c r="E169" s="4">
         <v>29</v>
@@ -36461,7 +36458,7 @@
         <v>3484</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>3919</v>
+        <v>3918</v>
       </c>
       <c r="E170" s="4">
         <v>71</v>
@@ -36481,7 +36478,7 @@
         <v>3485</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>3920</v>
+        <v>3919</v>
       </c>
       <c r="E171" s="4">
         <v>27</v>
@@ -36501,7 +36498,7 @@
         <v>3486</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>3921</v>
+        <v>3920</v>
       </c>
       <c r="E172" s="4">
         <v>18</v>
@@ -36521,7 +36518,7 @@
         <v>3487</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>3922</v>
+        <v>3921</v>
       </c>
       <c r="E173" s="4">
         <v>71</v>
@@ -36541,7 +36538,7 @@
         <v>3488</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>3923</v>
+        <v>3922</v>
       </c>
       <c r="E174" s="4">
         <v>70</v>
@@ -36561,7 +36558,7 @@
         <v>3489</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>3924</v>
+        <v>3923</v>
       </c>
       <c r="E175" s="4">
         <v>64</v>
@@ -36581,7 +36578,7 @@
         <v>3490</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>3925</v>
+        <v>3924</v>
       </c>
       <c r="E176" s="4">
         <v>61</v>
@@ -36601,7 +36598,7 @@
         <v>3491</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>3926</v>
+        <v>3925</v>
       </c>
       <c r="E177" s="4">
         <v>43</v>
@@ -36621,7 +36618,7 @@
         <v>3492</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>3927</v>
+        <v>3926</v>
       </c>
       <c r="E178" s="4">
         <v>38</v>
@@ -36641,7 +36638,7 @@
         <v>3493</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>3928</v>
+        <v>3927</v>
       </c>
       <c r="E179" s="4">
         <v>64</v>
@@ -36661,7 +36658,7 @@
         <v>3494</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>3929</v>
+        <v>3928</v>
       </c>
       <c r="E180" s="4">
         <v>77</v>
@@ -36681,7 +36678,7 @@
         <v>3495</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>3930</v>
+        <v>3929</v>
       </c>
       <c r="E181" s="4">
         <v>36</v>
@@ -36701,7 +36698,7 @@
         <v>3496</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>3931</v>
+        <v>3930</v>
       </c>
       <c r="E182" s="4">
         <v>80</v>
@@ -36721,7 +36718,7 @@
         <v>3497</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>3932</v>
+        <v>3931</v>
       </c>
       <c r="E183" s="4">
         <v>71</v>
@@ -36741,7 +36738,7 @@
         <v>3498</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>3933</v>
+        <v>3932</v>
       </c>
       <c r="E184" s="4">
         <v>76</v>
@@ -36761,7 +36758,7 @@
         <v>3499</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>3934</v>
+        <v>3933</v>
       </c>
       <c r="E185" s="4">
         <v>64</v>
@@ -36781,7 +36778,7 @@
         <v>3500</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>3935</v>
+        <v>3934</v>
       </c>
       <c r="E186" s="4">
         <v>17</v>
@@ -36801,7 +36798,7 @@
         <v>3501</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>3936</v>
+        <v>3935</v>
       </c>
       <c r="E187" s="4">
         <v>75</v>
@@ -36821,7 +36818,7 @@
         <v>3502</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>3937</v>
+        <v>3936</v>
       </c>
       <c r="E188" s="4">
         <v>15</v>
@@ -36841,7 +36838,7 @@
         <v>3503</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>3938</v>
+        <v>3937</v>
       </c>
       <c r="E189" s="4">
         <v>67</v>
@@ -36861,7 +36858,7 @@
         <v>3504</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>3939</v>
+        <v>3938</v>
       </c>
       <c r="E190" s="4">
         <v>68</v>
@@ -36881,7 +36878,7 @@
         <v>3505</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>3940</v>
+        <v>3939</v>
       </c>
       <c r="E191" s="4">
         <v>40</v>
@@ -36901,7 +36898,7 @@
         <v>3506</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>3941</v>
+        <v>3940</v>
       </c>
       <c r="E192" s="4">
         <v>49</v>
@@ -36921,7 +36918,7 @@
         <v>3507</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>3942</v>
+        <v>3941</v>
       </c>
       <c r="E193" s="4">
         <v>56</v>
@@ -36941,7 +36938,7 @@
         <v>3508</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>3943</v>
+        <v>3942</v>
       </c>
       <c r="E194" s="4">
         <v>2</v>
@@ -36961,7 +36958,7 @@
         <v>3509</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>3944</v>
+        <v>3943</v>
       </c>
       <c r="E195" s="4">
         <v>56</v>
@@ -36981,7 +36978,7 @@
         <v>3510</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>3945</v>
+        <v>3944</v>
       </c>
       <c r="E196" s="4">
         <v>11</v>
@@ -37001,7 +36998,7 @@
         <v>3511</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>3946</v>
+        <v>3945</v>
       </c>
       <c r="E197" s="4">
         <v>3</v>
@@ -37021,7 +37018,7 @@
         <v>3512</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>3947</v>
+        <v>3946</v>
       </c>
       <c r="E198" s="4">
         <v>67</v>
@@ -37041,7 +37038,7 @@
         <v>3513</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>3948</v>
+        <v>3947</v>
       </c>
       <c r="E199" s="4">
         <v>14</v>
@@ -37061,7 +37058,7 @@
         <v>3514</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>3949</v>
+        <v>3948</v>
       </c>
       <c r="E200" s="4">
         <v>30</v>
@@ -37081,7 +37078,7 @@
         <v>3515</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>3950</v>
+        <v>3949</v>
       </c>
       <c r="E201" s="4">
         <v>73</v>
@@ -37101,7 +37098,7 @@
         <v>3516</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>3951</v>
+        <v>3950</v>
       </c>
       <c r="E202" s="4">
         <v>80</v>
@@ -37121,7 +37118,7 @@
         <v>1245</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>3952</v>
+        <v>3951</v>
       </c>
       <c r="E203" s="4">
         <v>28</v>
@@ -37141,7 +37138,7 @@
         <v>3517</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>3953</v>
+        <v>3952</v>
       </c>
       <c r="E204" s="4">
         <v>13</v>
@@ -37161,7 +37158,7 @@
         <v>3518</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>3954</v>
+        <v>3953</v>
       </c>
       <c r="E205" s="4">
         <v>47</v>
@@ -37181,7 +37178,7 @@
         <v>3519</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>3955</v>
+        <v>3954</v>
       </c>
       <c r="E206" s="4">
         <v>52</v>
@@ -37201,7 +37198,7 @@
         <v>3520</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="E207" s="4">
         <v>25</v>
@@ -37221,7 +37218,7 @@
         <v>3521</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>3957</v>
+        <v>3956</v>
       </c>
       <c r="E208" s="4">
         <v>76</v>
@@ -37241,7 +37238,7 @@
         <v>3522</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>3958</v>
+        <v>3957</v>
       </c>
       <c r="E209" s="4">
         <v>10</v>
@@ -37261,7 +37258,7 @@
         <v>3523</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>3959</v>
+        <v>3958</v>
       </c>
       <c r="E210" s="4">
         <v>78</v>
@@ -37281,7 +37278,7 @@
         <v>3524</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>3960</v>
+        <v>3959</v>
       </c>
       <c r="E211" s="4">
         <v>34</v>
@@ -37301,7 +37298,7 @@
         <v>3525</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>3961</v>
+        <v>3960</v>
       </c>
       <c r="E212" s="4">
         <v>53</v>
@@ -37321,7 +37318,7 @@
         <v>3526</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>3962</v>
+        <v>3961</v>
       </c>
       <c r="E213" s="4">
         <v>29</v>
@@ -37341,7 +37338,7 @@
         <v>3527</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>3963</v>
+        <v>3962</v>
       </c>
       <c r="E214" s="4">
         <v>21</v>
@@ -37361,7 +37358,7 @@
         <v>3528</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>3964</v>
+        <v>3963</v>
       </c>
       <c r="E215" s="4">
         <v>30</v>
@@ -37381,7 +37378,7 @@
         <v>3529</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>3965</v>
+        <v>3964</v>
       </c>
       <c r="E216" s="4">
         <v>79</v>
@@ -37401,7 +37398,7 @@
         <v>3530</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>3966</v>
+        <v>3965</v>
       </c>
       <c r="E217" s="4">
         <v>77</v>
@@ -37421,7 +37418,7 @@
         <v>3531</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>3967</v>
+        <v>3966</v>
       </c>
       <c r="E218" s="4">
         <v>65</v>
@@ -37441,7 +37438,7 @@
         <v>3532</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>3968</v>
+        <v>3967</v>
       </c>
       <c r="E219" s="4">
         <v>2</v>
@@ -37461,7 +37458,7 @@
         <v>3533</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>3969</v>
+        <v>3968</v>
       </c>
       <c r="E220" s="4">
         <v>19</v>
@@ -37481,7 +37478,7 @@
         <v>3534</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>3970</v>
+        <v>3969</v>
       </c>
       <c r="E221" s="4">
         <v>1</v>
@@ -37501,7 +37498,7 @@
         <v>3535</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>3971</v>
+        <v>3970</v>
       </c>
       <c r="E222" s="4">
         <v>6</v>
@@ -37521,7 +37518,7 @@
         <v>3536</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>3972</v>
+        <v>3971</v>
       </c>
       <c r="E223" s="4">
         <v>62</v>
@@ -37541,7 +37538,7 @@
         <v>3537</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>3973</v>
+        <v>3972</v>
       </c>
       <c r="E224" s="4">
         <v>31</v>
@@ -37561,7 +37558,7 @@
         <v>3538</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>3974</v>
+        <v>3973</v>
       </c>
       <c r="E225" s="4">
         <v>7</v>
@@ -37581,7 +37578,7 @@
         <v>3539</v>
       </c>
       <c r="D226" s="4" t="s">
-        <v>3975</v>
+        <v>3974</v>
       </c>
       <c r="E226" s="4">
         <v>18</v>
@@ -37601,7 +37598,7 @@
         <v>3540</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>3976</v>
+        <v>3975</v>
       </c>
       <c r="E227" s="4">
         <v>46</v>
@@ -37621,7 +37618,7 @@
         <v>3541</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>3977</v>
+        <v>3976</v>
       </c>
       <c r="E228" s="4">
         <v>46</v>
@@ -37641,7 +37638,7 @@
         <v>3542</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>3978</v>
+        <v>3977</v>
       </c>
       <c r="E229" s="4">
         <v>33</v>
@@ -37661,7 +37658,7 @@
         <v>3543</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>3979</v>
+        <v>3978</v>
       </c>
       <c r="E230" s="4">
         <v>38</v>
@@ -37681,7 +37678,7 @@
         <v>3544</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>3980</v>
+        <v>3979</v>
       </c>
       <c r="E231" s="4">
         <v>79</v>
@@ -37701,7 +37698,7 @@
         <v>3545</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>3981</v>
+        <v>3980</v>
       </c>
       <c r="E232" s="4">
         <v>61</v>
@@ -37721,7 +37718,7 @@
         <v>3546</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="E233" s="4">
         <v>70</v>
@@ -37741,7 +37738,7 @@
         <v>3547</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>3983</v>
+        <v>3982</v>
       </c>
       <c r="E234" s="4">
         <v>45</v>
@@ -37761,7 +37758,7 @@
         <v>3548</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>3984</v>
+        <v>3983</v>
       </c>
       <c r="E235" s="4">
         <v>43</v>
@@ -37781,7 +37778,7 @@
         <v>3549</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>3985</v>
+        <v>3984</v>
       </c>
       <c r="E236" s="4">
         <v>17</v>
@@ -37801,7 +37798,7 @@
         <v>3550</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>3986</v>
+        <v>3985</v>
       </c>
       <c r="E237" s="4">
         <v>49</v>
@@ -37821,7 +37818,7 @@
         <v>3551</v>
       </c>
       <c r="D238" s="4" t="s">
-        <v>3987</v>
+        <v>3986</v>
       </c>
       <c r="E238" s="4">
         <v>32</v>
@@ -37841,7 +37838,7 @@
         <v>3552</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>3988</v>
+        <v>3987</v>
       </c>
       <c r="E239" s="4">
         <v>3</v>
@@ -37861,7 +37858,7 @@
         <v>3553</v>
       </c>
       <c r="D240" s="4" t="s">
-        <v>3989</v>
+        <v>3988</v>
       </c>
       <c r="E240" s="4">
         <v>41</v>
@@ -37881,7 +37878,7 @@
         <v>3554</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="E241" s="4">
         <v>9</v>
@@ -37901,7 +37898,7 @@
         <v>3555</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>3991</v>
+        <v>3990</v>
       </c>
       <c r="E242" s="4">
         <v>75</v>
@@ -37921,7 +37918,7 @@
         <v>3556</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="E243" s="4">
         <v>70</v>
@@ -37941,7 +37938,7 @@
         <v>3557</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>3993</v>
+        <v>3992</v>
       </c>
       <c r="E244" s="4">
         <v>78</v>
@@ -37961,7 +37958,7 @@
         <v>3558</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>3994</v>
+        <v>3993</v>
       </c>
       <c r="E245" s="4">
         <v>14</v>
@@ -37981,7 +37978,7 @@
         <v>3559</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>3995</v>
+        <v>3994</v>
       </c>
       <c r="E246" s="4">
         <v>22</v>
@@ -38001,7 +37998,7 @@
         <v>3560</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="E247" s="4">
         <v>20</v>
@@ -38021,7 +38018,7 @@
         <v>3561</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>3997</v>
+        <v>3996</v>
       </c>
       <c r="E248" s="4">
         <v>67</v>
@@ -38041,7 +38038,7 @@
         <v>3562</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="E249" s="4">
         <v>73</v>
@@ -38061,7 +38058,7 @@
         <v>3563</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="E250" s="4">
         <v>69</v>
@@ -38081,7 +38078,7 @@
         <v>3564</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="E251" s="4">
         <v>44</v>
@@ -38101,7 +38098,7 @@
         <v>3565</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="E252" s="4">
         <v>60</v>
@@ -38121,7 +38118,7 @@
         <v>3566</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="E253" s="4">
         <v>16</v>
@@ -38141,7 +38138,7 @@
         <v>3567</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>4003</v>
+        <v>4002</v>
       </c>
       <c r="E254" s="4">
         <v>40</v>
@@ -38161,7 +38158,7 @@
         <v>3568</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="E255" s="4">
         <v>75</v>
@@ -38181,7 +38178,7 @@
         <v>3569</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="E256" s="4">
         <v>27</v>
@@ -38201,7 +38198,7 @@
         <v>3570</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>4006</v>
+        <v>4005</v>
       </c>
       <c r="E257" s="4">
         <v>36</v>
@@ -38241,7 +38238,7 @@
         <v>3572</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="E259" s="4">
         <v>70</v>
@@ -38261,7 +38258,7 @@
         <v>3573</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>4008</v>
+        <v>4007</v>
       </c>
       <c r="E260" s="4">
         <v>58</v>
@@ -38281,7 +38278,7 @@
         <v>3574</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>4009</v>
+        <v>4008</v>
       </c>
       <c r="E261" s="4">
         <v>10</v>
@@ -38301,7 +38298,7 @@
         <v>3575</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>4010</v>
+        <v>4009</v>
       </c>
       <c r="E262" s="4">
         <v>54</v>
@@ -38321,7 +38318,7 @@
         <v>3576</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>4011</v>
+        <v>4010</v>
       </c>
       <c r="E263" s="4">
         <v>47</v>
@@ -38341,7 +38338,7 @@
         <v>3577</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>4012</v>
+        <v>4011</v>
       </c>
       <c r="E264" s="4">
         <v>21</v>
@@ -38361,7 +38358,7 @@
         <v>3578</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>4013</v>
+        <v>4012</v>
       </c>
       <c r="E265" s="4">
         <v>3</v>
@@ -38381,7 +38378,7 @@
         <v>3579</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>4014</v>
+        <v>4013</v>
       </c>
       <c r="E266" s="4">
         <v>24</v>
@@ -38401,7 +38398,7 @@
         <v>3580</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>4015</v>
+        <v>4014</v>
       </c>
       <c r="E267" s="4">
         <v>41</v>
@@ -38421,7 +38418,7 @@
         <v>3581</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>4016</v>
+        <v>4015</v>
       </c>
       <c r="E268" s="4">
         <v>46</v>
@@ -38441,7 +38438,7 @@
         <v>3582</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>4017</v>
+        <v>4016</v>
       </c>
       <c r="E269" s="4">
         <v>63</v>
@@ -38461,7 +38458,7 @@
         <v>3583</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>4018</v>
+        <v>4017</v>
       </c>
       <c r="E270" s="4">
         <v>61</v>
@@ -38481,7 +38478,7 @@
         <v>3584</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>4019</v>
+        <v>4018</v>
       </c>
       <c r="E271" s="4">
         <v>37</v>
@@ -38501,7 +38498,7 @@
         <v>3585</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>4020</v>
+        <v>4019</v>
       </c>
       <c r="E272" s="4">
         <v>58</v>
@@ -38521,7 +38518,7 @@
         <v>3586</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>4021</v>
+        <v>4020</v>
       </c>
       <c r="E273" s="4">
         <v>34</v>
@@ -38541,7 +38538,7 @@
         <v>3587</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>4022</v>
+        <v>4021</v>
       </c>
       <c r="E274" s="4">
         <v>51</v>
@@ -38561,7 +38558,7 @@
         <v>3588</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>4023</v>
+        <v>4022</v>
       </c>
       <c r="E275" s="4">
         <v>37</v>
@@ -38581,7 +38578,7 @@
         <v>3589</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>4024</v>
+        <v>4023</v>
       </c>
       <c r="E276" s="4">
         <v>11</v>
@@ -38601,7 +38598,7 @@
         <v>3590</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>4025</v>
+        <v>4024</v>
       </c>
       <c r="E277" s="4">
         <v>14</v>
@@ -38621,7 +38618,7 @@
         <v>3591</v>
       </c>
       <c r="D278" s="4" t="s">
-        <v>4026</v>
+        <v>4025</v>
       </c>
       <c r="E278" s="4">
         <v>50</v>
@@ -38641,7 +38638,7 @@
         <v>3592</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>4027</v>
+        <v>4026</v>
       </c>
       <c r="E279" s="4">
         <v>41</v>
@@ -38661,7 +38658,7 @@
         <v>3593</v>
       </c>
       <c r="D280" s="4" t="s">
-        <v>4028</v>
+        <v>4027</v>
       </c>
       <c r="E280" s="4">
         <v>60</v>
@@ -38681,7 +38678,7 @@
         <v>3594</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>4029</v>
+        <v>4028</v>
       </c>
       <c r="E281" s="4">
         <v>55</v>
@@ -38701,7 +38698,7 @@
         <v>3595</v>
       </c>
       <c r="D282" s="4" t="s">
-        <v>4030</v>
+        <v>4029</v>
       </c>
       <c r="E282" s="4">
         <v>18</v>
@@ -38721,7 +38718,7 @@
         <v>3596</v>
       </c>
       <c r="D283" s="4" t="s">
-        <v>4031</v>
+        <v>4030</v>
       </c>
       <c r="E283" s="4">
         <v>12</v>
@@ -38741,7 +38738,7 @@
         <v>3597</v>
       </c>
       <c r="D284" s="4" t="s">
-        <v>4032</v>
+        <v>4031</v>
       </c>
       <c r="E284" s="4">
         <v>21</v>
@@ -38761,7 +38758,7 @@
         <v>3598</v>
       </c>
       <c r="D285" s="4" t="s">
-        <v>4033</v>
+        <v>4032</v>
       </c>
       <c r="E285" s="4">
         <v>54</v>
@@ -38781,7 +38778,7 @@
         <v>3599</v>
       </c>
       <c r="D286" s="4" t="s">
-        <v>4034</v>
+        <v>4033</v>
       </c>
       <c r="E286" s="4">
         <v>53</v>
@@ -38801,7 +38798,7 @@
         <v>3600</v>
       </c>
       <c r="D287" s="4" t="s">
-        <v>4035</v>
+        <v>4034</v>
       </c>
       <c r="E287" s="4">
         <v>78</v>
@@ -38821,7 +38818,7 @@
         <v>3601</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>4036</v>
+        <v>4035</v>
       </c>
       <c r="E288" s="4">
         <v>20</v>
@@ -38841,7 +38838,7 @@
         <v>3602</v>
       </c>
       <c r="D289" s="4" t="s">
-        <v>4037</v>
+        <v>4036</v>
       </c>
       <c r="E289" s="4">
         <v>46</v>
@@ -38861,7 +38858,7 @@
         <v>3603</v>
       </c>
       <c r="D290" s="4" t="s">
-        <v>4038</v>
+        <v>4037</v>
       </c>
       <c r="E290" s="4">
         <v>18</v>
@@ -38881,7 +38878,7 @@
         <v>3604</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>4039</v>
+        <v>4038</v>
       </c>
       <c r="E291" s="4">
         <v>35</v>
@@ -38901,7 +38898,7 @@
         <v>3605</v>
       </c>
       <c r="D292" s="4" t="s">
-        <v>4040</v>
+        <v>4039</v>
       </c>
       <c r="E292" s="4">
         <v>52</v>
@@ -38921,7 +38918,7 @@
         <v>3606</v>
       </c>
       <c r="D293" s="4" t="s">
-        <v>4041</v>
+        <v>4040</v>
       </c>
       <c r="E293" s="4">
         <v>9</v>
@@ -38941,7 +38938,7 @@
         <v>3607</v>
       </c>
       <c r="D294" s="4" t="s">
-        <v>4042</v>
+        <v>4041</v>
       </c>
       <c r="E294" s="4">
         <v>40</v>
@@ -38961,7 +38958,7 @@
         <v>3608</v>
       </c>
       <c r="D295" s="4" t="s">
-        <v>4043</v>
+        <v>4042</v>
       </c>
       <c r="E295" s="4">
         <v>13</v>
@@ -38981,7 +38978,7 @@
         <v>3609</v>
       </c>
       <c r="D296" s="4" t="s">
-        <v>4044</v>
+        <v>4043</v>
       </c>
       <c r="E296" s="4">
         <v>69</v>
@@ -39001,7 +38998,7 @@
         <v>3610</v>
       </c>
       <c r="D297" s="4" t="s">
-        <v>4045</v>
+        <v>4044</v>
       </c>
       <c r="E297" s="4">
         <v>49</v>
@@ -39021,7 +39018,7 @@
         <v>3611</v>
       </c>
       <c r="D298" s="4" t="s">
-        <v>4046</v>
+        <v>4045</v>
       </c>
       <c r="E298" s="4">
         <v>52</v>
@@ -39041,7 +39038,7 @@
         <v>3612</v>
       </c>
       <c r="D299" s="4" t="s">
-        <v>4047</v>
+        <v>4046</v>
       </c>
       <c r="E299" s="4">
         <v>1</v>
@@ -39061,7 +39058,7 @@
         <v>3613</v>
       </c>
       <c r="D300" s="4" t="s">
-        <v>4048</v>
+        <v>4047</v>
       </c>
       <c r="E300" s="4">
         <v>70</v>
@@ -39081,7 +39078,7 @@
         <v>3614</v>
       </c>
       <c r="D301" s="4" t="s">
-        <v>4049</v>
+        <v>4048</v>
       </c>
       <c r="E301" s="4">
         <v>44</v>
@@ -39101,7 +39098,7 @@
         <v>3615</v>
       </c>
       <c r="D302" s="4" t="s">
-        <v>4050</v>
+        <v>4049</v>
       </c>
       <c r="E302" s="4">
         <v>1</v>
@@ -39121,7 +39118,7 @@
         <v>3616</v>
       </c>
       <c r="D303" s="4" t="s">
-        <v>4051</v>
+        <v>4050</v>
       </c>
       <c r="E303" s="4">
         <v>22</v>
@@ -39141,7 +39138,7 @@
         <v>3617</v>
       </c>
       <c r="D304" s="4" t="s">
-        <v>4052</v>
+        <v>4051</v>
       </c>
       <c r="E304" s="4">
         <v>13</v>
@@ -39161,7 +39158,7 @@
         <v>3618</v>
       </c>
       <c r="D305" s="4" t="s">
-        <v>4053</v>
+        <v>4052</v>
       </c>
       <c r="E305" s="4">
         <v>1</v>
@@ -39181,7 +39178,7 @@
         <v>3619</v>
       </c>
       <c r="D306" s="4" t="s">
-        <v>4054</v>
+        <v>4053</v>
       </c>
       <c r="E306" s="4">
         <v>55</v>
@@ -39201,7 +39198,7 @@
         <v>3620</v>
       </c>
       <c r="D307" s="4" t="s">
-        <v>4055</v>
+        <v>4054</v>
       </c>
       <c r="E307" s="4">
         <v>80</v>
@@ -39221,7 +39218,7 @@
         <v>3621</v>
       </c>
       <c r="D308" s="4" t="s">
-        <v>4056</v>
+        <v>4055</v>
       </c>
       <c r="E308" s="4">
         <v>2</v>
@@ -39241,7 +39238,7 @@
         <v>3622</v>
       </c>
       <c r="D309" s="4" t="s">
-        <v>4057</v>
+        <v>4056</v>
       </c>
       <c r="E309" s="4">
         <v>10</v>
@@ -39261,7 +39258,7 @@
         <v>3623</v>
       </c>
       <c r="D310" s="4" t="s">
-        <v>4058</v>
+        <v>4057</v>
       </c>
       <c r="E310" s="4">
         <v>48</v>
@@ -39281,7 +39278,7 @@
         <v>3624</v>
       </c>
       <c r="D311" s="4" t="s">
-        <v>4059</v>
+        <v>4058</v>
       </c>
       <c r="E311" s="4">
         <v>10</v>
@@ -39301,7 +39298,7 @@
         <v>3625</v>
       </c>
       <c r="D312" s="4" t="s">
-        <v>4060</v>
+        <v>4059</v>
       </c>
       <c r="E312" s="4">
         <v>4</v>
@@ -39321,7 +39318,7 @@
         <v>3626</v>
       </c>
       <c r="D313" s="4" t="s">
-        <v>4061</v>
+        <v>4060</v>
       </c>
       <c r="E313" s="4">
         <v>74</v>
@@ -39341,7 +39338,7 @@
         <v>3627</v>
       </c>
       <c r="D314" s="4" t="s">
-        <v>4062</v>
+        <v>4061</v>
       </c>
       <c r="E314" s="4">
         <v>4</v>
@@ -39361,7 +39358,7 @@
         <v>3628</v>
       </c>
       <c r="D315" s="4" t="s">
-        <v>4063</v>
+        <v>4062</v>
       </c>
       <c r="E315" s="4">
         <v>31</v>
@@ -39381,7 +39378,7 @@
         <v>3629</v>
       </c>
       <c r="D316" s="4" t="s">
-        <v>4064</v>
+        <v>4063</v>
       </c>
       <c r="E316" s="4">
         <v>14</v>
@@ -39401,7 +39398,7 @@
         <v>3630</v>
       </c>
       <c r="D317" s="4" t="s">
-        <v>4065</v>
+        <v>4064</v>
       </c>
       <c r="E317" s="4">
         <v>38</v>
@@ -39421,7 +39418,7 @@
         <v>3631</v>
       </c>
       <c r="D318" s="4" t="s">
-        <v>4066</v>
+        <v>4065</v>
       </c>
       <c r="E318" s="4">
         <v>50</v>
@@ -39441,7 +39438,7 @@
         <v>3632</v>
       </c>
       <c r="D319" s="4" t="s">
-        <v>4067</v>
+        <v>4066</v>
       </c>
       <c r="E319" s="4">
         <v>78</v>
@@ -39461,7 +39458,7 @@
         <v>3633</v>
       </c>
       <c r="D320" s="4" t="s">
-        <v>4068</v>
+        <v>4067</v>
       </c>
       <c r="E320" s="4">
         <v>65</v>
@@ -39481,7 +39478,7 @@
         <v>3634</v>
       </c>
       <c r="D321" s="4" t="s">
-        <v>4069</v>
+        <v>4068</v>
       </c>
       <c r="E321" s="4">
         <v>26</v>
@@ -39501,7 +39498,7 @@
         <v>3635</v>
       </c>
       <c r="D322" s="4" t="s">
-        <v>4070</v>
+        <v>4069</v>
       </c>
       <c r="E322" s="4">
         <v>57</v>
@@ -39521,7 +39518,7 @@
         <v>3636</v>
       </c>
       <c r="D323" s="4" t="s">
-        <v>4071</v>
+        <v>4070</v>
       </c>
       <c r="E323" s="4">
         <v>41</v>
@@ -39541,7 +39538,7 @@
         <v>3637</v>
       </c>
       <c r="D324" s="4" t="s">
-        <v>4072</v>
+        <v>4071</v>
       </c>
       <c r="E324" s="4">
         <v>29</v>
@@ -39561,7 +39558,7 @@
         <v>3638</v>
       </c>
       <c r="D325" s="4" t="s">
-        <v>4073</v>
+        <v>4072</v>
       </c>
       <c r="E325" s="4">
         <v>52</v>
@@ -39581,7 +39578,7 @@
         <v>3639</v>
       </c>
       <c r="D326" s="4" t="s">
-        <v>4074</v>
+        <v>4073</v>
       </c>
       <c r="E326" s="4">
         <v>8</v>
@@ -39601,7 +39598,7 @@
         <v>3640</v>
       </c>
       <c r="D327" s="4" t="s">
-        <v>4075</v>
+        <v>4074</v>
       </c>
       <c r="E327" s="4">
         <v>26</v>
@@ -39621,7 +39618,7 @@
         <v>3641</v>
       </c>
       <c r="D328" s="4" t="s">
-        <v>4076</v>
+        <v>4075</v>
       </c>
       <c r="E328" s="4">
         <v>49</v>
@@ -39641,7 +39638,7 @@
         <v>3642</v>
       </c>
       <c r="D329" s="4" t="s">
-        <v>4077</v>
+        <v>4076</v>
       </c>
       <c r="E329" s="4">
         <v>59</v>
@@ -39661,7 +39658,7 @@
         <v>3643</v>
       </c>
       <c r="D330" s="4" t="s">
-        <v>4078</v>
+        <v>4077</v>
       </c>
       <c r="E330" s="4">
         <v>69</v>
@@ -39681,7 +39678,7 @@
         <v>3644</v>
       </c>
       <c r="D331" s="4" t="s">
-        <v>4079</v>
+        <v>4078</v>
       </c>
       <c r="E331" s="4">
         <v>59</v>
@@ -39701,7 +39698,7 @@
         <v>3645</v>
       </c>
       <c r="D332" s="4" t="s">
-        <v>4080</v>
+        <v>4079</v>
       </c>
       <c r="E332" s="4">
         <v>2</v>
@@ -39721,7 +39718,7 @@
         <v>3646</v>
       </c>
       <c r="D333" s="4" t="s">
-        <v>4081</v>
+        <v>4080</v>
       </c>
       <c r="E333" s="4">
         <v>69</v>
@@ -39741,7 +39738,7 @@
         <v>3647</v>
       </c>
       <c r="D334" s="4" t="s">
-        <v>4082</v>
+        <v>4081</v>
       </c>
       <c r="E334" s="4">
         <v>80</v>
@@ -39761,7 +39758,7 @@
         <v>3648</v>
       </c>
       <c r="D335" s="4" t="s">
-        <v>4083</v>
+        <v>4082</v>
       </c>
       <c r="E335" s="4">
         <v>12</v>
@@ -39781,7 +39778,7 @@
         <v>3649</v>
       </c>
       <c r="D336" s="4" t="s">
-        <v>4084</v>
+        <v>4083</v>
       </c>
       <c r="E336" s="4">
         <v>11</v>
@@ -39801,7 +39798,7 @@
         <v>3650</v>
       </c>
       <c r="D337" s="4" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="E337" s="4">
         <v>8</v>
@@ -39821,7 +39818,7 @@
         <v>3651</v>
       </c>
       <c r="D338" s="4" t="s">
-        <v>4073</v>
+        <v>4072</v>
       </c>
       <c r="E338" s="4">
         <v>52</v>
@@ -39841,7 +39838,7 @@
         <v>3652</v>
       </c>
       <c r="D339" s="4" t="s">
-        <v>4086</v>
+        <v>4085</v>
       </c>
       <c r="E339" s="4">
         <v>36</v>
@@ -39861,7 +39858,7 @@
         <v>3653</v>
       </c>
       <c r="D340" s="4" t="s">
-        <v>4087</v>
+        <v>4086</v>
       </c>
       <c r="E340" s="4">
         <v>6</v>
@@ -39881,7 +39878,7 @@
         <v>3654</v>
       </c>
       <c r="D341" s="4" t="s">
-        <v>4088</v>
+        <v>4087</v>
       </c>
       <c r="E341" s="4">
         <v>25</v>
@@ -39901,7 +39898,7 @@
         <v>3655</v>
       </c>
       <c r="D342" s="4" t="s">
-        <v>4089</v>
+        <v>4088</v>
       </c>
       <c r="E342" s="4">
         <v>16</v>
@@ -39921,7 +39918,7 @@
         <v>3656</v>
       </c>
       <c r="D343" s="4" t="s">
-        <v>4090</v>
+        <v>4089</v>
       </c>
       <c r="E343" s="4">
         <v>3</v>
@@ -39941,7 +39938,7 @@
         <v>3657</v>
       </c>
       <c r="D344" s="4" t="s">
-        <v>4091</v>
+        <v>4090</v>
       </c>
       <c r="E344" s="4">
         <v>32</v>
@@ -39961,7 +39958,7 @@
         <v>3658</v>
       </c>
       <c r="D345" s="4" t="s">
-        <v>4092</v>
+        <v>4091</v>
       </c>
       <c r="E345" s="4">
         <v>57</v>
@@ -39981,7 +39978,7 @@
         <v>3659</v>
       </c>
       <c r="D346" s="4" t="s">
-        <v>4093</v>
+        <v>4092</v>
       </c>
       <c r="E346" s="4">
         <v>4</v>
@@ -40001,7 +39998,7 @@
         <v>3660</v>
       </c>
       <c r="D347" s="4" t="s">
-        <v>4094</v>
+        <v>4093</v>
       </c>
       <c r="E347" s="4">
         <v>74</v>
@@ -40021,7 +40018,7 @@
         <v>3661</v>
       </c>
       <c r="D348" s="4" t="s">
-        <v>4095</v>
+        <v>4094</v>
       </c>
       <c r="E348" s="4">
         <v>79</v>
@@ -40041,7 +40038,7 @@
         <v>3662</v>
       </c>
       <c r="D349" s="4" t="s">
-        <v>4096</v>
+        <v>4095</v>
       </c>
       <c r="E349" s="4">
         <v>55</v>
@@ -40061,7 +40058,7 @@
         <v>3663</v>
       </c>
       <c r="D350" s="4" t="s">
-        <v>4097</v>
+        <v>4096</v>
       </c>
       <c r="E350" s="4">
         <v>34</v>
@@ -40081,7 +40078,7 @@
         <v>3664</v>
       </c>
       <c r="D351" s="4" t="s">
-        <v>4098</v>
+        <v>4097</v>
       </c>
       <c r="E351" s="4">
         <v>43</v>
@@ -40101,7 +40098,7 @@
         <v>3665</v>
       </c>
       <c r="D352" s="4" t="s">
-        <v>4099</v>
+        <v>4098</v>
       </c>
       <c r="E352" s="4">
         <v>66</v>
@@ -40121,7 +40118,7 @@
         <v>1363</v>
       </c>
       <c r="D353" s="4" t="s">
-        <v>4100</v>
+        <v>4099</v>
       </c>
       <c r="E353" s="4">
         <v>29</v>
@@ -40141,7 +40138,7 @@
         <v>3666</v>
       </c>
       <c r="D354" s="4" t="s">
-        <v>4101</v>
+        <v>4100</v>
       </c>
       <c r="E354" s="4">
         <v>44</v>
@@ -40161,7 +40158,7 @@
         <v>3667</v>
       </c>
       <c r="D355" s="4" t="s">
-        <v>4102</v>
+        <v>4101</v>
       </c>
       <c r="E355" s="4">
         <v>40</v>
@@ -40181,7 +40178,7 @@
         <v>3668</v>
       </c>
       <c r="D356" s="4" t="s">
-        <v>4103</v>
+        <v>4102</v>
       </c>
       <c r="E356" s="4">
         <v>34</v>
@@ -40201,7 +40198,7 @@
         <v>3669</v>
       </c>
       <c r="D357" s="4" t="s">
-        <v>4104</v>
+        <v>4103</v>
       </c>
       <c r="E357" s="4">
         <v>47</v>
@@ -40221,7 +40218,7 @@
         <v>3670</v>
       </c>
       <c r="D358" s="4" t="s">
-        <v>4105</v>
+        <v>4104</v>
       </c>
       <c r="E358" s="4">
         <v>50</v>
@@ -40241,7 +40238,7 @@
         <v>3671</v>
       </c>
       <c r="D359" s="4" t="s">
-        <v>4106</v>
+        <v>4105</v>
       </c>
       <c r="E359" s="4">
         <v>75</v>
@@ -40261,7 +40258,7 @@
         <v>3672</v>
       </c>
       <c r="D360" s="4" t="s">
-        <v>4107</v>
+        <v>4106</v>
       </c>
       <c r="E360" s="4">
         <v>44</v>
@@ -40281,7 +40278,7 @@
         <v>3673</v>
       </c>
       <c r="D361" s="4" t="s">
-        <v>4108</v>
+        <v>4107</v>
       </c>
       <c r="E361" s="4">
         <v>63</v>
@@ -40301,7 +40298,7 @@
         <v>3674</v>
       </c>
       <c r="D362" s="4" t="s">
-        <v>4109</v>
+        <v>4108</v>
       </c>
       <c r="E362" s="4">
         <v>45</v>
@@ -40321,7 +40318,7 @@
         <v>3675</v>
       </c>
       <c r="D363" s="4" t="s">
-        <v>4110</v>
+        <v>4109</v>
       </c>
       <c r="E363" s="4">
         <v>58</v>
@@ -40341,7 +40338,7 @@
         <v>3676</v>
       </c>
       <c r="D364" s="4" t="s">
-        <v>4111</v>
+        <v>4110</v>
       </c>
       <c r="E364" s="4">
         <v>61</v>
@@ -40361,7 +40358,7 @@
         <v>3677</v>
       </c>
       <c r="D365" s="4" t="s">
-        <v>4112</v>
+        <v>4111</v>
       </c>
       <c r="E365" s="4">
         <v>64</v>
@@ -40381,7 +40378,7 @@
         <v>3678</v>
       </c>
       <c r="D366" s="4" t="s">
-        <v>4113</v>
+        <v>4112</v>
       </c>
       <c r="E366" s="4">
         <v>79</v>
@@ -40401,7 +40398,7 @@
         <v>3679</v>
       </c>
       <c r="D367" s="4" t="s">
-        <v>4114</v>
+        <v>4113</v>
       </c>
       <c r="E367" s="4">
         <v>70</v>
@@ -40421,7 +40418,7 @@
         <v>3680</v>
       </c>
       <c r="D368" s="4" t="s">
-        <v>4115</v>
+        <v>4114</v>
       </c>
       <c r="E368" s="4">
         <v>79</v>
@@ -40441,7 +40438,7 @@
         <v>3681</v>
       </c>
       <c r="D369" s="4" t="s">
-        <v>4116</v>
+        <v>4115</v>
       </c>
       <c r="E369" s="4">
         <v>4</v>
@@ -40461,7 +40458,7 @@
         <v>3682</v>
       </c>
       <c r="D370" s="4" t="s">
-        <v>4117</v>
+        <v>4116</v>
       </c>
       <c r="E370" s="4">
         <v>1</v>
@@ -40481,7 +40478,7 @@
         <v>3683</v>
       </c>
       <c r="D371" s="4" t="s">
-        <v>4118</v>
+        <v>4117</v>
       </c>
       <c r="E371" s="4">
         <v>75</v>
@@ -40501,7 +40498,7 @@
         <v>3684</v>
       </c>
       <c r="D372" s="4" t="s">
-        <v>4119</v>
+        <v>4118</v>
       </c>
       <c r="E372" s="4">
         <v>49</v>
@@ -40521,7 +40518,7 @@
         <v>3685</v>
       </c>
       <c r="D373" s="4" t="s">
-        <v>4120</v>
+        <v>4119</v>
       </c>
       <c r="E373" s="4">
         <v>33</v>
@@ -40541,7 +40538,7 @@
         <v>3686</v>
       </c>
       <c r="D374" s="4" t="s">
-        <v>4121</v>
+        <v>4120</v>
       </c>
       <c r="E374" s="4">
         <v>2</v>
@@ -40561,7 +40558,7 @@
         <v>3687</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>4122</v>
+        <v>4121</v>
       </c>
       <c r="E375" s="4">
         <v>5</v>
@@ -40581,7 +40578,7 @@
         <v>3688</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>4123</v>
+        <v>4122</v>
       </c>
       <c r="E376" s="4">
         <v>73</v>
@@ -40601,7 +40598,7 @@
         <v>3689</v>
       </c>
       <c r="D377" s="4" t="s">
-        <v>4124</v>
+        <v>4123</v>
       </c>
       <c r="E377" s="4">
         <v>17</v>
@@ -40621,7 +40618,7 @@
         <v>3690</v>
       </c>
       <c r="D378" s="4" t="s">
-        <v>4125</v>
+        <v>4124</v>
       </c>
       <c r="E378" s="4">
         <v>56</v>
@@ -40641,7 +40638,7 @@
         <v>3691</v>
       </c>
       <c r="D379" s="4" t="s">
-        <v>4126</v>
+        <v>4125</v>
       </c>
       <c r="E379" s="4">
         <v>79</v>
@@ -40661,7 +40658,7 @@
         <v>3692</v>
       </c>
       <c r="D380" s="4" t="s">
-        <v>4127</v>
+        <v>4126</v>
       </c>
       <c r="E380" s="4">
         <v>42</v>
@@ -40681,7 +40678,7 @@
         <v>3693</v>
       </c>
       <c r="D381" s="4" t="s">
-        <v>4128</v>
+        <v>4127</v>
       </c>
       <c r="E381" s="4">
         <v>28</v>
@@ -40701,7 +40698,7 @@
         <v>3694</v>
       </c>
       <c r="D382" s="4" t="s">
-        <v>4129</v>
+        <v>4128</v>
       </c>
       <c r="E382" s="4">
         <v>5</v>
@@ -40721,7 +40718,7 @@
         <v>3695</v>
       </c>
       <c r="D383" s="4" t="s">
-        <v>4130</v>
+        <v>4129</v>
       </c>
       <c r="E383" s="4">
         <v>58</v>
@@ -40741,7 +40738,7 @@
         <v>3696</v>
       </c>
       <c r="D384" s="4" t="s">
-        <v>4131</v>
+        <v>4130</v>
       </c>
       <c r="E384" s="4">
         <v>75</v>
@@ -40761,7 +40758,7 @@
         <v>1919</v>
       </c>
       <c r="D385" s="4" t="s">
-        <v>4132</v>
+        <v>4131</v>
       </c>
       <c r="E385" s="4">
         <v>52</v>
@@ -40801,7 +40798,7 @@
         <v>3698</v>
       </c>
       <c r="D387" s="4" t="s">
-        <v>4133</v>
+        <v>4132</v>
       </c>
       <c r="E387" s="4">
         <v>38</v>
@@ -40821,7 +40818,7 @@
         <v>3699</v>
       </c>
       <c r="D388" s="4" t="s">
-        <v>4134</v>
+        <v>4133</v>
       </c>
       <c r="E388" s="4">
         <v>72</v>
@@ -40841,7 +40838,7 @@
         <v>3700</v>
       </c>
       <c r="D389" s="4" t="s">
-        <v>4135</v>
+        <v>4134</v>
       </c>
       <c r="E389" s="4">
         <v>30</v>
@@ -40861,7 +40858,7 @@
         <v>3701</v>
       </c>
       <c r="D390" s="4" t="s">
-        <v>4136</v>
+        <v>4135</v>
       </c>
       <c r="E390" s="4">
         <v>40</v>
@@ -40881,7 +40878,7 @@
         <v>3702</v>
       </c>
       <c r="D391" s="4" t="s">
-        <v>4137</v>
+        <v>4136</v>
       </c>
       <c r="E391" s="4">
         <v>42</v>
@@ -40901,7 +40898,7 @@
         <v>3703</v>
       </c>
       <c r="D392" s="4" t="s">
-        <v>4138</v>
+        <v>4137</v>
       </c>
       <c r="E392" s="4">
         <v>16</v>
@@ -40921,7 +40918,7 @@
         <v>3704</v>
       </c>
       <c r="D393" s="4" t="s">
-        <v>4139</v>
+        <v>4138</v>
       </c>
       <c r="E393" s="4">
         <v>48</v>
@@ -40941,7 +40938,7 @@
         <v>3705</v>
       </c>
       <c r="D394" s="4" t="s">
-        <v>4140</v>
+        <v>4139</v>
       </c>
       <c r="E394" s="4">
         <v>44</v>
@@ -40961,7 +40958,7 @@
         <v>3706</v>
       </c>
       <c r="D395" s="4" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="E395" s="4">
         <v>34</v>
@@ -40981,7 +40978,7 @@
         <v>3707</v>
       </c>
       <c r="D396" s="4" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
       <c r="E396" s="4">
         <v>18</v>
@@ -41001,7 +40998,7 @@
         <v>3708</v>
       </c>
       <c r="D397" s="4" t="s">
-        <v>4143</v>
+        <v>4142</v>
       </c>
       <c r="E397" s="4">
         <v>17</v>
@@ -41021,7 +41018,7 @@
         <v>3709</v>
       </c>
       <c r="D398" s="4" t="s">
-        <v>4144</v>
+        <v>4143</v>
       </c>
       <c r="E398" s="4">
         <v>16</v>
@@ -41041,7 +41038,7 @@
         <v>3710</v>
       </c>
       <c r="D399" s="4" t="s">
-        <v>4145</v>
+        <v>4144</v>
       </c>
       <c r="E399" s="4">
         <v>66</v>
@@ -41061,7 +41058,7 @@
         <v>3711</v>
       </c>
       <c r="D400" s="4" t="s">
-        <v>4146</v>
+        <v>4145</v>
       </c>
       <c r="E400" s="4">
         <v>71</v>
@@ -41081,7 +41078,7 @@
         <v>3712</v>
       </c>
       <c r="D401" s="4" t="s">
-        <v>4147</v>
+        <v>4146</v>
       </c>
       <c r="E401" s="4">
         <v>23</v>

</xml_diff>